<commit_message>
Added Tutorial VIdeo Link
</commit_message>
<xml_diff>
--- a/Runtime Performance Testing.xlsx
+++ b/Runtime Performance Testing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chand\Documents\SPU\3430 Algorithm Design and Analysis\Small-Groups-Algorithm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chand\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD464A0B-6FBA-4C1C-B941-BACB6A91CCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E878A2DE-96F1-402A-89A0-E8AEAD824574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,12 +140,20 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Showing O(n^3) Time Complexity (Trendline equation:                                                 )</a:t>
+              <a:t>Showing O(n^3) Time Complexity (Trendline equation:                                                  )</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26551610789442587"/>
+          <c:y val="1.5231399590221382E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -248,8 +256,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.26613005911778076"/>
-                  <c:y val="-0.10207031599607282"/>
+                  <c:x val="-0.26222828558435651"/>
+                  <c:y val="-0.14858230300260958"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -876,583 +884,583 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="193"/>
                 <c:pt idx="0">
-                  <c:v>1033.8999999999901</c:v>
+                  <c:v>39692.400000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1480.19999999999</c:v>
+                  <c:v>54212.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2039.8999999999901</c:v>
+                  <c:v>58479.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1942.8999999999901</c:v>
+                  <c:v>69173.899999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3018.8</c:v>
+                  <c:v>84810.499999999898</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2909.4</c:v>
+                  <c:v>79709.899999999805</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3559.0999999999899</c:v>
+                  <c:v>89622.499999999898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9127.6</c:v>
+                  <c:v>91223.799999999799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7134.9</c:v>
+                  <c:v>112279.299999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6813.1</c:v>
+                  <c:v>150378.29999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6542.7000000000098</c:v>
+                  <c:v>164497.70000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9567.6999999999898</c:v>
+                  <c:v>176355.1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9958.8999999999905</c:v>
+                  <c:v>177023.9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10211.9</c:v>
+                  <c:v>178341.799999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12037.4</c:v>
+                  <c:v>178713.9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15737.5999999999</c:v>
+                  <c:v>179776.3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21372.5</c:v>
+                  <c:v>180154.6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16595.2</c:v>
+                  <c:v>181985.899999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>28258.999999999902</c:v>
+                  <c:v>182797.8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>28524.7</c:v>
+                  <c:v>183804.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25942.999999999902</c:v>
+                  <c:v>184339.4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>23450.2</c:v>
+                  <c:v>185315.799999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>25099.499999999902</c:v>
+                  <c:v>186502.59999999899</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>27290.499999999902</c:v>
+                  <c:v>187740.79999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>34557.1</c:v>
+                  <c:v>188591.3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41805.599999999999</c:v>
+                  <c:v>189846.899999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>60569.5</c:v>
+                  <c:v>190254.09999999899</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43048.099999999897</c:v>
+                  <c:v>195865.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>47159.999999999898</c:v>
+                  <c:v>221498.3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>45064.6</c:v>
+                  <c:v>226208.69999999899</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>62097.999999999898</c:v>
+                  <c:v>235662.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>75151.899999999907</c:v>
+                  <c:v>241222.8</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>79434.699999999895</c:v>
+                  <c:v>267483.69999999902</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>85686.300000000105</c:v>
+                  <c:v>281724.50000000099</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>93036.699999999793</c:v>
+                  <c:v>286288.50000000099</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>78490.799999999901</c:v>
+                  <c:v>296811.99999999901</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>84538.199999999895</c:v>
+                  <c:v>309269.8</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>94827.8</c:v>
+                  <c:v>322245.50000000099</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>97192.6</c:v>
+                  <c:v>343083.3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>100502.499999999</c:v>
+                  <c:v>328403.39999999898</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>139668.6</c:v>
+                  <c:v>376494.99999999802</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>111751.099999999</c:v>
+                  <c:v>395889.09999999899</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>125401.999999999</c:v>
+                  <c:v>400973.8</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>120101.299999999</c:v>
+                  <c:v>416458.99999999901</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>166028.4</c:v>
+                  <c:v>461456.49999999802</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>201676.79999999999</c:v>
+                  <c:v>462421.7</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>245793.799999999</c:v>
+                  <c:v>498112.7</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>229403.6</c:v>
+                  <c:v>485175.8</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>250625.799999999</c:v>
+                  <c:v>518328.9</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>168367.299999999</c:v>
+                  <c:v>552708.69999999995</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>173591.59999999899</c:v>
+                  <c:v>548015.69999999797</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>186318.7</c:v>
+                  <c:v>582816.19999999995</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>185071.69999999899</c:v>
+                  <c:v>545544.59999999905</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>192148.299999999</c:v>
+                  <c:v>666986.99999999802</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>238279.2</c:v>
+                  <c:v>648236.19999999902</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>217601</c:v>
+                  <c:v>632115.69999999995</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>249037.2</c:v>
+                  <c:v>728130.69999999704</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>258330</c:v>
+                  <c:v>699598.8</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>287037.99999999901</c:v>
+                  <c:v>764413.2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>269395.59999999899</c:v>
+                  <c:v>777583.19999999797</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>314228.09999999998</c:v>
+                  <c:v>845687.69999999902</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>327299.40000000002</c:v>
+                  <c:v>860421.89999999804</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>310606.90000000002</c:v>
+                  <c:v>896229.69999999902</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>326301.799999999</c:v>
+                  <c:v>907466.699999996</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>341061.59999999899</c:v>
+                  <c:v>947838.099999998</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>418730.09999999899</c:v>
+                  <c:v>946529.00000000105</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>358922.4</c:v>
+                  <c:v>981071.6</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>426588.39999999898</c:v>
+                  <c:v>984228.599999998</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>425059.59999999899</c:v>
+                  <c:v>1133890.8999999899</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>539029.19999999902</c:v>
+                  <c:v>1142227.6999999899</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>490262.90000000101</c:v>
+                  <c:v>1164444.3999999999</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>474846.49999999901</c:v>
+                  <c:v>1172516.3999999899</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>476015.9</c:v>
+                  <c:v>1227772.99999999</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>523966.1</c:v>
+                  <c:v>1329425.49999999</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>483662.1</c:v>
+                  <c:v>1327387.6000000001</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>509489.99999999901</c:v>
+                  <c:v>1291615.8</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>557096.099999998</c:v>
+                  <c:v>1391124.9</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>574028.10000000102</c:v>
+                  <c:v>1412541.6999999899</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>569890.6</c:v>
+                  <c:v>1462636.5999999901</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>598476.09999999905</c:v>
+                  <c:v>1498009.4</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>657605.39999999898</c:v>
+                  <c:v>1510719.6999999899</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>671600.89999999001</c:v>
+                  <c:v>1582781.1999999899</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>732725.19999999797</c:v>
+                  <c:v>1664942.29999999</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>724154</c:v>
+                  <c:v>1705819.5999999901</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>808246.700000001</c:v>
+                  <c:v>1749921.2</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>824873.9</c:v>
+                  <c:v>1876557.29999999</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>834984.900000002</c:v>
+                  <c:v>1854825.0999999901</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>838343.400000002</c:v>
+                  <c:v>1815064.49999999</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>850283.09999998996</c:v>
+                  <c:v>1961748.4</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>869166.10000000102</c:v>
+                  <c:v>1962225.4</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>909444.3</c:v>
+                  <c:v>2020744.4</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>925925.59999999905</c:v>
+                  <c:v>2031531.29999999</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>995928.89999999898</c:v>
+                  <c:v>2148300.3999999901</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1052689.8999999999</c:v>
+                  <c:v>2198111.5999999898</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1049997.3</c:v>
+                  <c:v>2210924.9</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1036860.9</c:v>
+                  <c:v>2200067.7000000002</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1077151.79999999</c:v>
+                  <c:v>2272951.3999999901</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1088146.3999999899</c:v>
+                  <c:v>2398748.6</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1137677</c:v>
+                  <c:v>2428849.29999999</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1168616.8999999999</c:v>
+                  <c:v>2461067.9999999902</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1168126.8999999999</c:v>
+                  <c:v>2535324.2000000002</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1207100.1999999899</c:v>
+                  <c:v>2651283.7999999998</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1233706.29999999</c:v>
+                  <c:v>2672443</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1243617.6000000001</c:v>
+                  <c:v>2694007.0999999898</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1317923.3999999999</c:v>
+                  <c:v>2777874.1</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1302547.6999999899</c:v>
+                  <c:v>2919085.1999999899</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1376072.49999999</c:v>
+                  <c:v>3145995.9</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1407719.7</c:v>
+                  <c:v>3134020.3999999901</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1402665.3</c:v>
+                  <c:v>3116739.4</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1565260.8</c:v>
+                  <c:v>3208402.5999999898</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>1606338.29999999</c:v>
+                  <c:v>3251885.8999999901</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1776677.0999999901</c:v>
+                  <c:v>3322990</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1755644.6999999899</c:v>
+                  <c:v>3385336.8999999901</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1625925.5</c:v>
+                  <c:v>3448094.8</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1689992.7</c:v>
+                  <c:v>3583501.79999997</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>1728826.49999999</c:v>
+                  <c:v>3588736.79999999</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1708238.8999999899</c:v>
+                  <c:v>3818869.4999999702</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>1863514.1999999899</c:v>
+                  <c:v>3804555.8999999901</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>2098660.1</c:v>
+                  <c:v>3825064.1999999802</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>2082087.6</c:v>
+                  <c:v>3795803.3000000101</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>1953972.29999998</c:v>
+                  <c:v>4176180.1000000099</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>1959285.99999999</c:v>
+                  <c:v>4244549.9000000097</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>2075448.6</c:v>
+                  <c:v>4246403.8000000203</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>2134735.2000000002</c:v>
+                  <c:v>4301416.8999999901</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2120804.8999999901</c:v>
+                  <c:v>4423427.2000000197</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>2173059.6999999899</c:v>
+                  <c:v>4503332.1999999797</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>2296125.3999999901</c:v>
+                  <c:v>4672865.0999999903</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>2388838.1999999899</c:v>
+                  <c:v>4604205.7999999803</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>2451977.5999999898</c:v>
+                  <c:v>4771044.3</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>2420346.70000001</c:v>
+                  <c:v>4908068.9999999804</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>2345516.9</c:v>
+                  <c:v>5027897.7000000104</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>2427792.6999999899</c:v>
+                  <c:v>5042427.5</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>2578954.5</c:v>
+                  <c:v>5200085.3999999696</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>2655378.6</c:v>
+                  <c:v>5331335.3</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>2670403.1</c:v>
+                  <c:v>5334495.2000000197</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>2701474.8999999901</c:v>
+                  <c:v>5329344.8</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>2704250.0999999898</c:v>
+                  <c:v>5447038.3999999901</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>3021074.0999999898</c:v>
+                  <c:v>5659362.5</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>2905607.5999999898</c:v>
+                  <c:v>5761351.9000000199</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>2953529.5999999898</c:v>
+                  <c:v>5701784.2000000197</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>2994561.0999999898</c:v>
+                  <c:v>5984038.9000000004</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>3227109.3999999799</c:v>
+                  <c:v>5967934.3999999901</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>3327432.8999999901</c:v>
+                  <c:v>6097968.2000000197</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>3240396.5</c:v>
+                  <c:v>6329842.9999999804</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>3206707.6</c:v>
+                  <c:v>6381144.1999999899</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>3261764.9999999902</c:v>
+                  <c:v>6529486.8999999901</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>3230801.29999999</c:v>
+                  <c:v>6496083.8999999696</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>3301657.6000000201</c:v>
+                  <c:v>6894610.6000000201</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>3422429.6</c:v>
+                  <c:v>7054006.5000000102</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>3501433.1000000201</c:v>
+                  <c:v>7033023.8999999799</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>3604718.7</c:v>
+                  <c:v>7062499</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>3572834.2999999798</c:v>
+                  <c:v>7209161.6000000099</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>3657133.7</c:v>
+                  <c:v>7326084.3999999501</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>3952496.9</c:v>
+                  <c:v>7552212.1000000201</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>4025324.1</c:v>
+                  <c:v>7692412.4000000199</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>4097904.70000001</c:v>
+                  <c:v>7353521.2000000402</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>4280928.9999999804</c:v>
+                  <c:v>8203989.2999999896</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>4306900.8999999799</c:v>
+                  <c:v>7932902.0000000102</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>4531690.9000000004</c:v>
+                  <c:v>8022478.7000000197</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>4566246.4999999702</c:v>
+                  <c:v>8107298.8000000203</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>4358962.6000000099</c:v>
+                  <c:v>8262117.1000000099</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>4666608.0999999903</c:v>
+                  <c:v>8690883.5999999996</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>4699375.7999999803</c:v>
+                  <c:v>8738655.6000000108</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>4935294.7000000104</c:v>
+                  <c:v>8747068.1999999993</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>5093192.2999999896</c:v>
+                  <c:v>9404311</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>5017999.5999999903</c:v>
+                  <c:v>9142753.7000000104</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>4887808.4000000097</c:v>
+                  <c:v>9245289.6999999993</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>4740849.9999999898</c:v>
+                  <c:v>9459108.4000000004</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>4934391.7999999803</c:v>
+                  <c:v>9677914.1999999695</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>5278683.9999999898</c:v>
+                  <c:v>9661172.5999999791</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>4989233.9000000097</c:v>
+                  <c:v>9795158.7999999598</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>5036985.1000000099</c:v>
+                  <c:v>10646563.499999899</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>5182567.3</c:v>
+                  <c:v>10254324.9</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>5321435.5999999801</c:v>
+                  <c:v>10349599.300000001</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>5565437.3999999603</c:v>
+                  <c:v>10264845.8999999</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>5638436.2000000002</c:v>
+                  <c:v>10586106.7999999</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>5685797.1999999601</c:v>
+                  <c:v>10741498.6</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>5704311.6999999704</c:v>
+                  <c:v>11558590.199999999</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>5724623.6000000099</c:v>
+                  <c:v>11251881.2999999</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>5874014.0999999698</c:v>
+                  <c:v>11115566.2000001</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>5916888.4999999804</c:v>
+                  <c:v>11559944.800000001</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>6093081.2999999998</c:v>
+                  <c:v>11600588.6</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>6220902.3999999799</c:v>
+                  <c:v>11619943.1</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>6338315.0000000196</c:v>
+                  <c:v>12527725.999999899</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>6568465.8999999696</c:v>
+                  <c:v>12090112.699999901</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>6414334.2999999998</c:v>
+                  <c:v>12301635.499999899</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>6998769.5999999996</c:v>
+                  <c:v>12556515.300000001</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>6887075.4000000097</c:v>
+                  <c:v>12559081.699999901</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>6823485.6000000201</c:v>
+                  <c:v>13519775.099999901</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>7489242.7999999998</c:v>
+                  <c:v>13172470.199999999</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>7178853.6999999899</c:v>
+                  <c:v>13362788.499999899</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>7324386.0999999698</c:v>
+                  <c:v>13347540.199999999</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>7493329.5999999801</c:v>
+                  <c:v>13777049.699999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3329,9 +3337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3353,7 +3359,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>1033.8999999999901</v>
+        <v>39692.400000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3361,7 +3367,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>1480.19999999999</v>
+        <v>54212.7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3369,7 +3375,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>2039.8999999999901</v>
+        <v>58479.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3377,7 +3383,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>1942.8999999999901</v>
+        <v>69173.899999999994</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3385,7 +3391,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>3018.8</v>
+        <v>84810.499999999898</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3393,7 +3399,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>2909.4</v>
+        <v>79709.899999999805</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3401,7 +3407,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>3559.0999999999899</v>
+        <v>89622.499999999898</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3409,7 +3415,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>9127.6</v>
+        <v>91223.799999999799</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3417,7 +3423,7 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>7134.9</v>
+        <v>112279.299999999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3425,7 +3431,7 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>6813.1</v>
+        <v>150378.29999999999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3433,7 +3439,7 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>6542.7000000000098</v>
+        <v>164497.70000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3441,7 +3447,7 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>9567.6999999999898</v>
+        <v>176355.1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3449,7 +3455,7 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>9958.8999999999905</v>
+        <v>177023.9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3457,7 +3463,7 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>10211.9</v>
+        <v>178341.799999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3465,7 +3471,7 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>12037.4</v>
+        <v>178713.9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3473,7 +3479,7 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>15737.5999999999</v>
+        <v>179776.3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3481,7 +3487,7 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <v>21372.5</v>
+        <v>180154.6</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3489,7 +3495,7 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <v>16595.2</v>
+        <v>181985.899999999</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3497,7 +3503,7 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>28258.999999999902</v>
+        <v>182797.8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3505,7 +3511,7 @@
         <v>27</v>
       </c>
       <c r="B21">
-        <v>28524.7</v>
+        <v>183804.2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3513,7 +3519,7 @@
         <v>28</v>
       </c>
       <c r="B22">
-        <v>25942.999999999902</v>
+        <v>184339.4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3521,7 +3527,7 @@
         <v>29</v>
       </c>
       <c r="B23">
-        <v>23450.2</v>
+        <v>185315.799999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3529,7 +3535,7 @@
         <v>30</v>
       </c>
       <c r="B24">
-        <v>25099.499999999902</v>
+        <v>186502.59999999899</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3537,7 +3543,7 @@
         <v>31</v>
       </c>
       <c r="B25">
-        <v>27290.499999999902</v>
+        <v>187740.79999999999</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3545,7 +3551,7 @@
         <v>32</v>
       </c>
       <c r="B26">
-        <v>34557.1</v>
+        <v>188591.3</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3553,7 +3559,7 @@
         <v>33</v>
       </c>
       <c r="B27">
-        <v>41805.599999999999</v>
+        <v>189846.899999999</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3561,7 +3567,7 @@
         <v>34</v>
       </c>
       <c r="B28">
-        <v>60569.5</v>
+        <v>190254.09999999899</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3569,7 +3575,7 @@
         <v>35</v>
       </c>
       <c r="B29">
-        <v>43048.099999999897</v>
+        <v>195865.5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -3577,7 +3583,7 @@
         <v>36</v>
       </c>
       <c r="B30">
-        <v>47159.999999999898</v>
+        <v>221498.3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -3585,7 +3591,7 @@
         <v>37</v>
       </c>
       <c r="B31">
-        <v>45064.6</v>
+        <v>226208.69999999899</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3593,7 +3599,7 @@
         <v>38</v>
       </c>
       <c r="B32">
-        <v>62097.999999999898</v>
+        <v>235662.5</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3601,7 +3607,7 @@
         <v>39</v>
       </c>
       <c r="B33">
-        <v>75151.899999999907</v>
+        <v>241222.8</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3609,7 +3615,7 @@
         <v>40</v>
       </c>
       <c r="B34">
-        <v>79434.699999999895</v>
+        <v>267483.69999999902</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3617,7 +3623,7 @@
         <v>41</v>
       </c>
       <c r="B35">
-        <v>85686.300000000105</v>
+        <v>281724.50000000099</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3625,7 +3631,7 @@
         <v>42</v>
       </c>
       <c r="B36">
-        <v>93036.699999999793</v>
+        <v>286288.50000000099</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3633,7 +3639,7 @@
         <v>43</v>
       </c>
       <c r="B37">
-        <v>78490.799999999901</v>
+        <v>296811.99999999901</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3641,7 +3647,7 @@
         <v>44</v>
       </c>
       <c r="B38">
-        <v>84538.199999999895</v>
+        <v>309269.8</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -3649,7 +3655,7 @@
         <v>45</v>
       </c>
       <c r="B39">
-        <v>94827.8</v>
+        <v>322245.50000000099</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -3657,7 +3663,7 @@
         <v>46</v>
       </c>
       <c r="B40">
-        <v>97192.6</v>
+        <v>343083.3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3665,7 +3671,7 @@
         <v>47</v>
       </c>
       <c r="B41">
-        <v>100502.499999999</v>
+        <v>328403.39999999898</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3673,7 +3679,7 @@
         <v>48</v>
       </c>
       <c r="B42">
-        <v>139668.6</v>
+        <v>376494.99999999802</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3681,7 +3687,7 @@
         <v>49</v>
       </c>
       <c r="B43">
-        <v>111751.099999999</v>
+        <v>395889.09999999899</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -3689,7 +3695,7 @@
         <v>50</v>
       </c>
       <c r="B44">
-        <v>125401.999999999</v>
+        <v>400973.8</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3697,7 +3703,7 @@
         <v>51</v>
       </c>
       <c r="B45">
-        <v>120101.299999999</v>
+        <v>416458.99999999901</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3705,7 +3711,7 @@
         <v>52</v>
       </c>
       <c r="B46">
-        <v>166028.4</v>
+        <v>461456.49999999802</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3713,7 +3719,7 @@
         <v>53</v>
       </c>
       <c r="B47">
-        <v>201676.79999999999</v>
+        <v>462421.7</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3721,7 +3727,7 @@
         <v>54</v>
       </c>
       <c r="B48">
-        <v>245793.799999999</v>
+        <v>498112.7</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3729,7 +3735,7 @@
         <v>55</v>
       </c>
       <c r="B49">
-        <v>229403.6</v>
+        <v>485175.8</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3737,7 +3743,7 @@
         <v>56</v>
       </c>
       <c r="B50">
-        <v>250625.799999999</v>
+        <v>518328.9</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3745,7 +3751,7 @@
         <v>57</v>
       </c>
       <c r="B51">
-        <v>168367.299999999</v>
+        <v>552708.69999999995</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3753,7 +3759,7 @@
         <v>58</v>
       </c>
       <c r="B52">
-        <v>173591.59999999899</v>
+        <v>548015.69999999797</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3761,7 +3767,7 @@
         <v>59</v>
       </c>
       <c r="B53">
-        <v>186318.7</v>
+        <v>582816.19999999995</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -3769,7 +3775,7 @@
         <v>60</v>
       </c>
       <c r="B54">
-        <v>185071.69999999899</v>
+        <v>545544.59999999905</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -3777,7 +3783,7 @@
         <v>61</v>
       </c>
       <c r="B55">
-        <v>192148.299999999</v>
+        <v>666986.99999999802</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -3785,7 +3791,7 @@
         <v>62</v>
       </c>
       <c r="B56">
-        <v>238279.2</v>
+        <v>648236.19999999902</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -3793,7 +3799,7 @@
         <v>63</v>
       </c>
       <c r="B57">
-        <v>217601</v>
+        <v>632115.69999999995</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -3801,7 +3807,7 @@
         <v>64</v>
       </c>
       <c r="B58">
-        <v>249037.2</v>
+        <v>728130.69999999704</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3809,7 +3815,7 @@
         <v>65</v>
       </c>
       <c r="B59">
-        <v>258330</v>
+        <v>699598.8</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -3817,7 +3823,7 @@
         <v>66</v>
       </c>
       <c r="B60">
-        <v>287037.99999999901</v>
+        <v>764413.2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3825,7 +3831,7 @@
         <v>67</v>
       </c>
       <c r="B61">
-        <v>269395.59999999899</v>
+        <v>777583.19999999797</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3833,7 +3839,7 @@
         <v>68</v>
       </c>
       <c r="B62">
-        <v>314228.09999999998</v>
+        <v>845687.69999999902</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3841,7 +3847,7 @@
         <v>69</v>
       </c>
       <c r="B63">
-        <v>327299.40000000002</v>
+        <v>860421.89999999804</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -3849,7 +3855,7 @@
         <v>70</v>
       </c>
       <c r="B64">
-        <v>310606.90000000002</v>
+        <v>896229.69999999902</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -3857,7 +3863,7 @@
         <v>71</v>
       </c>
       <c r="B65">
-        <v>326301.799999999</v>
+        <v>907466.699999996</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -3865,7 +3871,7 @@
         <v>72</v>
       </c>
       <c r="B66">
-        <v>341061.59999999899</v>
+        <v>947838.099999998</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -3873,7 +3879,7 @@
         <v>73</v>
       </c>
       <c r="B67">
-        <v>418730.09999999899</v>
+        <v>946529.00000000105</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -3881,7 +3887,7 @@
         <v>74</v>
       </c>
       <c r="B68">
-        <v>358922.4</v>
+        <v>981071.6</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -3889,7 +3895,7 @@
         <v>75</v>
       </c>
       <c r="B69">
-        <v>426588.39999999898</v>
+        <v>984228.599999998</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -3897,7 +3903,7 @@
         <v>76</v>
       </c>
       <c r="B70">
-        <v>425059.59999999899</v>
+        <v>1133890.8999999899</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -3905,7 +3911,7 @@
         <v>77</v>
       </c>
       <c r="B71">
-        <v>539029.19999999902</v>
+        <v>1142227.6999999899</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -3913,7 +3919,7 @@
         <v>78</v>
       </c>
       <c r="B72">
-        <v>490262.90000000101</v>
+        <v>1164444.3999999999</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -3921,7 +3927,7 @@
         <v>79</v>
       </c>
       <c r="B73">
-        <v>474846.49999999901</v>
+        <v>1172516.3999999899</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -3929,7 +3935,7 @@
         <v>80</v>
       </c>
       <c r="B74">
-        <v>476015.9</v>
+        <v>1227772.99999999</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -3937,7 +3943,7 @@
         <v>81</v>
       </c>
       <c r="B75">
-        <v>523966.1</v>
+        <v>1329425.49999999</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -3945,7 +3951,7 @@
         <v>82</v>
       </c>
       <c r="B76">
-        <v>483662.1</v>
+        <v>1327387.6000000001</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -3953,7 +3959,7 @@
         <v>83</v>
       </c>
       <c r="B77">
-        <v>509489.99999999901</v>
+        <v>1291615.8</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -3961,7 +3967,7 @@
         <v>84</v>
       </c>
       <c r="B78">
-        <v>557096.099999998</v>
+        <v>1391124.9</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -3969,7 +3975,7 @@
         <v>85</v>
       </c>
       <c r="B79">
-        <v>574028.10000000102</v>
+        <v>1412541.6999999899</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -3977,7 +3983,7 @@
         <v>86</v>
       </c>
       <c r="B80">
-        <v>569890.6</v>
+        <v>1462636.5999999901</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -3985,7 +3991,7 @@
         <v>87</v>
       </c>
       <c r="B81">
-        <v>598476.09999999905</v>
+        <v>1498009.4</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -3993,7 +3999,7 @@
         <v>88</v>
       </c>
       <c r="B82">
-        <v>657605.39999999898</v>
+        <v>1510719.6999999899</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -4001,7 +4007,7 @@
         <v>89</v>
       </c>
       <c r="B83">
-        <v>671600.89999999001</v>
+        <v>1582781.1999999899</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -4009,7 +4015,7 @@
         <v>90</v>
       </c>
       <c r="B84">
-        <v>732725.19999999797</v>
+        <v>1664942.29999999</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -4017,7 +4023,7 @@
         <v>91</v>
       </c>
       <c r="B85">
-        <v>724154</v>
+        <v>1705819.5999999901</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -4025,7 +4031,7 @@
         <v>92</v>
       </c>
       <c r="B86">
-        <v>808246.700000001</v>
+        <v>1749921.2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -4033,7 +4039,7 @@
         <v>93</v>
       </c>
       <c r="B87">
-        <v>824873.9</v>
+        <v>1876557.29999999</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -4041,7 +4047,7 @@
         <v>94</v>
       </c>
       <c r="B88">
-        <v>834984.900000002</v>
+        <v>1854825.0999999901</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -4049,7 +4055,7 @@
         <v>95</v>
       </c>
       <c r="B89">
-        <v>838343.400000002</v>
+        <v>1815064.49999999</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -4057,7 +4063,7 @@
         <v>96</v>
       </c>
       <c r="B90">
-        <v>850283.09999998996</v>
+        <v>1961748.4</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -4065,7 +4071,7 @@
         <v>97</v>
       </c>
       <c r="B91">
-        <v>869166.10000000102</v>
+        <v>1962225.4</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -4073,7 +4079,7 @@
         <v>98</v>
       </c>
       <c r="B92">
-        <v>909444.3</v>
+        <v>2020744.4</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -4081,7 +4087,7 @@
         <v>99</v>
       </c>
       <c r="B93">
-        <v>925925.59999999905</v>
+        <v>2031531.29999999</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -4089,7 +4095,7 @@
         <v>100</v>
       </c>
       <c r="B94">
-        <v>995928.89999999898</v>
+        <v>2148300.3999999901</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -4097,7 +4103,7 @@
         <v>101</v>
       </c>
       <c r="B95">
-        <v>1052689.8999999999</v>
+        <v>2198111.5999999898</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -4105,7 +4111,7 @@
         <v>102</v>
       </c>
       <c r="B96">
-        <v>1049997.3</v>
+        <v>2210924.9</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -4113,7 +4119,7 @@
         <v>103</v>
       </c>
       <c r="B97">
-        <v>1036860.9</v>
+        <v>2200067.7000000002</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -4121,7 +4127,7 @@
         <v>104</v>
       </c>
       <c r="B98">
-        <v>1077151.79999999</v>
+        <v>2272951.3999999901</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -4129,7 +4135,7 @@
         <v>105</v>
       </c>
       <c r="B99">
-        <v>1088146.3999999899</v>
+        <v>2398748.6</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -4137,7 +4143,7 @@
         <v>106</v>
       </c>
       <c r="B100">
-        <v>1137677</v>
+        <v>2428849.29999999</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -4145,7 +4151,7 @@
         <v>107</v>
       </c>
       <c r="B101">
-        <v>1168616.8999999999</v>
+        <v>2461067.9999999902</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -4153,7 +4159,7 @@
         <v>108</v>
       </c>
       <c r="B102">
-        <v>1168126.8999999999</v>
+        <v>2535324.2000000002</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -4161,7 +4167,7 @@
         <v>109</v>
       </c>
       <c r="B103">
-        <v>1207100.1999999899</v>
+        <v>2651283.7999999998</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -4169,7 +4175,7 @@
         <v>110</v>
       </c>
       <c r="B104">
-        <v>1233706.29999999</v>
+        <v>2672443</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -4177,7 +4183,7 @@
         <v>111</v>
       </c>
       <c r="B105">
-        <v>1243617.6000000001</v>
+        <v>2694007.0999999898</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -4185,7 +4191,7 @@
         <v>112</v>
       </c>
       <c r="B106">
-        <v>1317923.3999999999</v>
+        <v>2777874.1</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -4193,7 +4199,7 @@
         <v>113</v>
       </c>
       <c r="B107">
-        <v>1302547.6999999899</v>
+        <v>2919085.1999999899</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -4201,7 +4207,7 @@
         <v>114</v>
       </c>
       <c r="B108">
-        <v>1376072.49999999</v>
+        <v>3145995.9</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -4209,7 +4215,7 @@
         <v>115</v>
       </c>
       <c r="B109">
-        <v>1407719.7</v>
+        <v>3134020.3999999901</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -4217,7 +4223,7 @@
         <v>116</v>
       </c>
       <c r="B110">
-        <v>1402665.3</v>
+        <v>3116739.4</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -4225,7 +4231,7 @@
         <v>117</v>
       </c>
       <c r="B111">
-        <v>1565260.8</v>
+        <v>3208402.5999999898</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -4233,7 +4239,7 @@
         <v>118</v>
       </c>
       <c r="B112">
-        <v>1606338.29999999</v>
+        <v>3251885.8999999901</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -4241,7 +4247,7 @@
         <v>119</v>
       </c>
       <c r="B113">
-        <v>1776677.0999999901</v>
+        <v>3322990</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -4249,7 +4255,7 @@
         <v>120</v>
       </c>
       <c r="B114">
-        <v>1755644.6999999899</v>
+        <v>3385336.8999999901</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -4257,7 +4263,7 @@
         <v>121</v>
       </c>
       <c r="B115">
-        <v>1625925.5</v>
+        <v>3448094.8</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -4265,7 +4271,7 @@
         <v>122</v>
       </c>
       <c r="B116">
-        <v>1689992.7</v>
+        <v>3583501.79999997</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -4273,7 +4279,7 @@
         <v>123</v>
       </c>
       <c r="B117">
-        <v>1728826.49999999</v>
+        <v>3588736.79999999</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -4281,7 +4287,7 @@
         <v>124</v>
       </c>
       <c r="B118">
-        <v>1708238.8999999899</v>
+        <v>3818869.4999999702</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -4289,7 +4295,7 @@
         <v>125</v>
       </c>
       <c r="B119">
-        <v>1863514.1999999899</v>
+        <v>3804555.8999999901</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -4297,7 +4303,7 @@
         <v>126</v>
       </c>
       <c r="B120">
-        <v>2098660.1</v>
+        <v>3825064.1999999802</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -4305,7 +4311,7 @@
         <v>127</v>
       </c>
       <c r="B121">
-        <v>2082087.6</v>
+        <v>3795803.3000000101</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -4313,7 +4319,7 @@
         <v>128</v>
       </c>
       <c r="B122">
-        <v>1953972.29999998</v>
+        <v>4176180.1000000099</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -4321,7 +4327,7 @@
         <v>129</v>
       </c>
       <c r="B123">
-        <v>1959285.99999999</v>
+        <v>4244549.9000000097</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -4329,7 +4335,7 @@
         <v>130</v>
       </c>
       <c r="B124">
-        <v>2075448.6</v>
+        <v>4246403.8000000203</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -4337,7 +4343,7 @@
         <v>131</v>
       </c>
       <c r="B125">
-        <v>2134735.2000000002</v>
+        <v>4301416.8999999901</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -4345,7 +4351,7 @@
         <v>132</v>
       </c>
       <c r="B126">
-        <v>2120804.8999999901</v>
+        <v>4423427.2000000197</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -4353,7 +4359,7 @@
         <v>133</v>
       </c>
       <c r="B127">
-        <v>2173059.6999999899</v>
+        <v>4503332.1999999797</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -4361,7 +4367,7 @@
         <v>134</v>
       </c>
       <c r="B128">
-        <v>2296125.3999999901</v>
+        <v>4672865.0999999903</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -4369,7 +4375,7 @@
         <v>135</v>
       </c>
       <c r="B129">
-        <v>2388838.1999999899</v>
+        <v>4604205.7999999803</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -4377,7 +4383,7 @@
         <v>136</v>
       </c>
       <c r="B130">
-        <v>2451977.5999999898</v>
+        <v>4771044.3</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -4385,7 +4391,7 @@
         <v>137</v>
       </c>
       <c r="B131">
-        <v>2420346.70000001</v>
+        <v>4908068.9999999804</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -4393,7 +4399,7 @@
         <v>138</v>
       </c>
       <c r="B132">
-        <v>2345516.9</v>
+        <v>5027897.7000000104</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -4401,7 +4407,7 @@
         <v>139</v>
       </c>
       <c r="B133">
-        <v>2427792.6999999899</v>
+        <v>5042427.5</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -4409,7 +4415,7 @@
         <v>140</v>
       </c>
       <c r="B134">
-        <v>2578954.5</v>
+        <v>5200085.3999999696</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -4417,7 +4423,7 @@
         <v>141</v>
       </c>
       <c r="B135">
-        <v>2655378.6</v>
+        <v>5331335.3</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -4425,7 +4431,7 @@
         <v>142</v>
       </c>
       <c r="B136">
-        <v>2670403.1</v>
+        <v>5334495.2000000197</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -4433,7 +4439,7 @@
         <v>143</v>
       </c>
       <c r="B137">
-        <v>2701474.8999999901</v>
+        <v>5329344.8</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -4441,7 +4447,7 @@
         <v>144</v>
       </c>
       <c r="B138">
-        <v>2704250.0999999898</v>
+        <v>5447038.3999999901</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -4449,7 +4455,7 @@
         <v>145</v>
       </c>
       <c r="B139">
-        <v>3021074.0999999898</v>
+        <v>5659362.5</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -4457,7 +4463,7 @@
         <v>146</v>
       </c>
       <c r="B140">
-        <v>2905607.5999999898</v>
+        <v>5761351.9000000199</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -4465,7 +4471,7 @@
         <v>147</v>
       </c>
       <c r="B141">
-        <v>2953529.5999999898</v>
+        <v>5701784.2000000197</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -4473,7 +4479,7 @@
         <v>148</v>
       </c>
       <c r="B142">
-        <v>2994561.0999999898</v>
+        <v>5984038.9000000004</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -4481,7 +4487,7 @@
         <v>149</v>
       </c>
       <c r="B143">
-        <v>3227109.3999999799</v>
+        <v>5967934.3999999901</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -4489,7 +4495,7 @@
         <v>150</v>
       </c>
       <c r="B144">
-        <v>3327432.8999999901</v>
+        <v>6097968.2000000197</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -4497,7 +4503,7 @@
         <v>151</v>
       </c>
       <c r="B145">
-        <v>3240396.5</v>
+        <v>6329842.9999999804</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -4505,7 +4511,7 @@
         <v>152</v>
       </c>
       <c r="B146">
-        <v>3206707.6</v>
+        <v>6381144.1999999899</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -4513,7 +4519,7 @@
         <v>153</v>
       </c>
       <c r="B147">
-        <v>3261764.9999999902</v>
+        <v>6529486.8999999901</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -4521,7 +4527,7 @@
         <v>154</v>
       </c>
       <c r="B148">
-        <v>3230801.29999999</v>
+        <v>6496083.8999999696</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -4529,7 +4535,7 @@
         <v>155</v>
       </c>
       <c r="B149">
-        <v>3301657.6000000201</v>
+        <v>6894610.6000000201</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -4537,7 +4543,7 @@
         <v>156</v>
       </c>
       <c r="B150">
-        <v>3422429.6</v>
+        <v>7054006.5000000102</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -4545,7 +4551,7 @@
         <v>157</v>
       </c>
       <c r="B151">
-        <v>3501433.1000000201</v>
+        <v>7033023.8999999799</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -4553,7 +4559,7 @@
         <v>158</v>
       </c>
       <c r="B152">
-        <v>3604718.7</v>
+        <v>7062499</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -4561,7 +4567,7 @@
         <v>159</v>
       </c>
       <c r="B153">
-        <v>3572834.2999999798</v>
+        <v>7209161.6000000099</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -4569,7 +4575,7 @@
         <v>160</v>
       </c>
       <c r="B154">
-        <v>3657133.7</v>
+        <v>7326084.3999999501</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -4577,7 +4583,7 @@
         <v>161</v>
       </c>
       <c r="B155">
-        <v>3952496.9</v>
+        <v>7552212.1000000201</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -4585,7 +4591,7 @@
         <v>162</v>
       </c>
       <c r="B156">
-        <v>4025324.1</v>
+        <v>7692412.4000000199</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -4593,7 +4599,7 @@
         <v>163</v>
       </c>
       <c r="B157">
-        <v>4097904.70000001</v>
+        <v>7353521.2000000402</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -4601,7 +4607,7 @@
         <v>164</v>
       </c>
       <c r="B158">
-        <v>4280928.9999999804</v>
+        <v>8203989.2999999896</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -4609,7 +4615,7 @@
         <v>165</v>
       </c>
       <c r="B159">
-        <v>4306900.8999999799</v>
+        <v>7932902.0000000102</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -4617,7 +4623,7 @@
         <v>166</v>
       </c>
       <c r="B160">
-        <v>4531690.9000000004</v>
+        <v>8022478.7000000197</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -4625,7 +4631,7 @@
         <v>167</v>
       </c>
       <c r="B161">
-        <v>4566246.4999999702</v>
+        <v>8107298.8000000203</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -4633,7 +4639,7 @@
         <v>168</v>
       </c>
       <c r="B162">
-        <v>4358962.6000000099</v>
+        <v>8262117.1000000099</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -4641,7 +4647,7 @@
         <v>169</v>
       </c>
       <c r="B163">
-        <v>4666608.0999999903</v>
+        <v>8690883.5999999996</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -4649,7 +4655,7 @@
         <v>170</v>
       </c>
       <c r="B164">
-        <v>4699375.7999999803</v>
+        <v>8738655.6000000108</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -4657,7 +4663,7 @@
         <v>171</v>
       </c>
       <c r="B165">
-        <v>4935294.7000000104</v>
+        <v>8747068.1999999993</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -4665,7 +4671,7 @@
         <v>172</v>
       </c>
       <c r="B166">
-        <v>5093192.2999999896</v>
+        <v>9404311</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -4673,7 +4679,7 @@
         <v>173</v>
       </c>
       <c r="B167">
-        <v>5017999.5999999903</v>
+        <v>9142753.7000000104</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -4681,7 +4687,7 @@
         <v>174</v>
       </c>
       <c r="B168">
-        <v>4887808.4000000097</v>
+        <v>9245289.6999999993</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -4689,7 +4695,7 @@
         <v>175</v>
       </c>
       <c r="B169">
-        <v>4740849.9999999898</v>
+        <v>9459108.4000000004</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -4697,7 +4703,7 @@
         <v>176</v>
       </c>
       <c r="B170">
-        <v>4934391.7999999803</v>
+        <v>9677914.1999999695</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -4705,7 +4711,7 @@
         <v>177</v>
       </c>
       <c r="B171">
-        <v>5278683.9999999898</v>
+        <v>9661172.5999999791</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -4713,7 +4719,7 @@
         <v>178</v>
       </c>
       <c r="B172">
-        <v>4989233.9000000097</v>
+        <v>9795158.7999999598</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -4721,7 +4727,7 @@
         <v>179</v>
       </c>
       <c r="B173">
-        <v>5036985.1000000099</v>
+        <v>10646563.499999899</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -4729,7 +4735,7 @@
         <v>180</v>
       </c>
       <c r="B174">
-        <v>5182567.3</v>
+        <v>10254324.9</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -4737,7 +4743,7 @@
         <v>181</v>
       </c>
       <c r="B175">
-        <v>5321435.5999999801</v>
+        <v>10349599.300000001</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -4745,7 +4751,7 @@
         <v>182</v>
       </c>
       <c r="B176">
-        <v>5565437.3999999603</v>
+        <v>10264845.8999999</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -4753,7 +4759,7 @@
         <v>183</v>
       </c>
       <c r="B177">
-        <v>5638436.2000000002</v>
+        <v>10586106.7999999</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -4761,7 +4767,7 @@
         <v>184</v>
       </c>
       <c r="B178">
-        <v>5685797.1999999601</v>
+        <v>10741498.6</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -4769,7 +4775,7 @@
         <v>185</v>
       </c>
       <c r="B179">
-        <v>5704311.6999999704</v>
+        <v>11558590.199999999</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -4777,7 +4783,7 @@
         <v>186</v>
       </c>
       <c r="B180">
-        <v>5724623.6000000099</v>
+        <v>11251881.2999999</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -4785,7 +4791,7 @@
         <v>187</v>
       </c>
       <c r="B181">
-        <v>5874014.0999999698</v>
+        <v>11115566.2000001</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -4793,7 +4799,7 @@
         <v>188</v>
       </c>
       <c r="B182">
-        <v>5916888.4999999804</v>
+        <v>11559944.800000001</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -4801,7 +4807,7 @@
         <v>189</v>
       </c>
       <c r="B183">
-        <v>6093081.2999999998</v>
+        <v>11600588.6</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -4809,7 +4815,7 @@
         <v>190</v>
       </c>
       <c r="B184">
-        <v>6220902.3999999799</v>
+        <v>11619943.1</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -4817,7 +4823,7 @@
         <v>191</v>
       </c>
       <c r="B185">
-        <v>6338315.0000000196</v>
+        <v>12527725.999999899</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -4825,7 +4831,7 @@
         <v>192</v>
       </c>
       <c r="B186">
-        <v>6568465.8999999696</v>
+        <v>12090112.699999901</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -4833,7 +4839,7 @@
         <v>193</v>
       </c>
       <c r="B187">
-        <v>6414334.2999999998</v>
+        <v>12301635.499999899</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -4841,7 +4847,7 @@
         <v>194</v>
       </c>
       <c r="B188">
-        <v>6998769.5999999996</v>
+        <v>12556515.300000001</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -4849,7 +4855,7 @@
         <v>195</v>
       </c>
       <c r="B189">
-        <v>6887075.4000000097</v>
+        <v>12559081.699999901</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -4857,7 +4863,7 @@
         <v>196</v>
       </c>
       <c r="B190">
-        <v>6823485.6000000201</v>
+        <v>13519775.099999901</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -4865,7 +4871,7 @@
         <v>197</v>
       </c>
       <c r="B191">
-        <v>7489242.7999999998</v>
+        <v>13172470.199999999</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -4873,7 +4879,7 @@
         <v>198</v>
       </c>
       <c r="B192">
-        <v>7178853.6999999899</v>
+        <v>13362788.499999899</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -4881,7 +4887,7 @@
         <v>199</v>
       </c>
       <c r="B193">
-        <v>7324386.0999999698</v>
+        <v>13347540.199999999</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -4889,7 +4895,7 @@
         <v>200</v>
       </c>
       <c r="B194">
-        <v>7493329.5999999801</v>
+        <v>13777049.699999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>